<commit_message>
Added noloop rxn essentiality
</commit_message>
<xml_diff>
--- a/Flux_Variability/table 2_11012016.xlsx
+++ b/Flux_Variability/table 2_11012016.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="245">
   <si>
     <t>Model 1</t>
   </si>
@@ -1187,16 +1187,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1789,42 +1789,42 @@
   <sheetData>
     <row r="2" spans="1:325" ht="16.2" thickBot="1"/>
     <row r="3" spans="1:325">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64" t="s">
+      <c r="E3" s="63"/>
+      <c r="F3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="63"/>
       <c r="H3" s="35"/>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64" t="s">
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64" t="s">
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64" t="s">
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
       <c r="U3" s="29"/>
       <c r="V3" s="29"/>
       <c r="W3" s="29"/>
@@ -2132,7 +2132,7 @@
       <c r="LM3" s="29"/>
     </row>
     <row r="4" spans="1:325" ht="49.8" thickBot="1">
-      <c r="A4" s="63"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="41" t="s">
         <v>11</v>
       </c>
@@ -3268,26 +3268,26 @@
       </c>
     </row>
     <row r="19" spans="2:20" s="19" customFormat="1">
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="65"/>
-      <c r="R19" s="65"/>
-      <c r="S19" s="65"/>
-      <c r="T19" s="65"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
     </row>
     <row r="20" spans="2:20" s="19" customFormat="1">
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
       <c r="K20" s="22"/>
@@ -3406,6 +3406,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:K3"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
@@ -3416,11 +3421,6 @@
     <mergeCell ref="O19:Q19"/>
     <mergeCell ref="R19:T19"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3534,42 +3534,42 @@
   <sheetData>
     <row r="2" spans="1:325" ht="16.2" thickBot="1"/>
     <row r="3" spans="1:325">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64" t="s">
+      <c r="E3" s="63"/>
+      <c r="F3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="63"/>
       <c r="H3" s="35"/>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64" t="s">
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64" t="s">
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64" t="s">
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
       <c r="U3" s="29"/>
       <c r="V3" s="29"/>
       <c r="W3" s="29"/>
@@ -3877,7 +3877,7 @@
       <c r="LM3" s="29"/>
     </row>
     <row r="4" spans="1:325" ht="49.8" thickBot="1">
-      <c r="A4" s="63"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="41" t="s">
         <v>11</v>
       </c>
@@ -5008,26 +5008,26 @@
       </c>
     </row>
     <row r="19" spans="2:20" s="19" customFormat="1">
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="65"/>
-      <c r="R19" s="65"/>
-      <c r="S19" s="65"/>
-      <c r="T19" s="65"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
     </row>
     <row r="20" spans="2:20" s="19" customFormat="1">
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
       <c r="K20" s="22"/>
@@ -5143,6 +5143,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
@@ -5151,13 +5158,6 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6163,6 +6163,12 @@
     <sortCondition ref="B25:B32"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="L21:N21"/>
@@ -6171,12 +6177,6 @@
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11296,7 +11296,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A36"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -11307,6 +11307,7 @@
     <col min="12" max="13" width="10.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -12669,8 +12670,36 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
+      <c r="A37" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="G37" s="61">
+        <v>0</v>
+      </c>
+      <c r="H37" s="61">
+        <v>0</v>
+      </c>
+      <c r="K37" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="L37" s="61">
+        <v>0</v>
+      </c>
+      <c r="M37" s="61">
+        <v>0</v>
+      </c>
+      <c r="P37" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q37" s="56">
+        <v>-41.7</v>
+      </c>
+      <c r="R37" s="56">
+        <v>-41.7</v>
+      </c>
     </row>
     <row r="38" spans="1:18">
       <c r="B38" s="59"/>

</xml_diff>